<commit_message>
Committed on 27:02:2018:01:05:00AM By Karthikeyan Rajendran
</commit_message>
<xml_diff>
--- a/data/Mail_Campaign_One.xlsx
+++ b/data/Mail_Campaign_One.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="8385" windowWidth="20385"/>
+    <workbookView windowHeight="8385" windowWidth="20385" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="196">
   <si>
     <t>Email ID</t>
   </si>
@@ -335,6 +335,366 @@
   </si>
   <si>
     <t>agoldberg@advisorsplus.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if mhillenbrand@advisorsplus.com
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if brink@alvinailey.org
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>tcott@alvinailey.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>ian.coulson@ajbell.com is not
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>j.shevchenko@alpha-dent.net is not
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if alex.smith@altech.com
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if robert.venter@altech.com
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>craig@alternateenergyhawaii.com is not
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>mike@alternateenergyhawaii.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>jeffcarroll88@aol.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if bschiff@alvarezandmarsal.com
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if rbaker@alvarezandmarsal.com
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if gabrielle@alzforum.org
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if tfagan@alzforum.org
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if tclifford@amalcap.com
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>racedirector@americandogderby.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>rhonda@americandogderby.com is not
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if bbeggs@americantrademagazines.com
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>cthompson@atmags.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if cthompson@americantrademagazines.com
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if ireid@anaqua.com
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if jmorgan@anaqua.com
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if amy.evans@andersonsmiles.com
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>president@ania.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if mburton@aof.org
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if sdowney@aof.org
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if rawbery@apcap.com
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>heidi.benedum@apisoftwareinc.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>caguilera@aplaviation.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if kurt_kwok@appliedmaterials.com
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if shannon.phillips@appliedmaterials.com
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if schwerdtfeger@arc-energy.com
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if ullal@arc-energy.com
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>Jett@mail.wvu.edu is not
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if lkurowski@feldinc.com
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if TFerguson@feldinc.com
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if andrew.annandale@argentaplc.com
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if david.powell@argentaplc.com
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if dave@arportastor.com
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if jnordlinger@ascentsg.com
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if mmiller@ascentsg.com
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>cschonberg@ashtonwoods.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>brad.shaffer@ucla.edu is not
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>maxphoto@earthlink.net is not
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>lenzcap@aol.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>okristensen@aurasound.com is not
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>pandreyev@aurasound.com is not
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if dcrane@austinlivingonline.com
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>Avana522lease@greystar.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>mklier@azdvs.gov is not
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>tvogt@azdvs.gov is not
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>michael.trailor@azhousing.gov is not
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>mscorca@azopera.org is not
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if michelle@bankbement.com
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if tabitha@bankbement.com
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>editor@banner-tribune.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>m.roggasch@bracpet.com is not
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if jaybayer@bayerbecker.com
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if roger@beaverstateins.com
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>robynd@becnet.org is not
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if amir@beholdisrael.com
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dluck@belladomicile.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>wditzler@beloitlibrary.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>candybz@gmail.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>kathybigda@mapinternet.com is not
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>rkuypers@newwhey.com is not
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if mteichman@bethelhebrew.org
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if president@bethelhebrew.org
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>amy@bezansonitsolutions.com is not
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>dosman@cj.com is not
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if president@bhcpr.org
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if henderson@bioagrimix.com
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>chairman@bluepilotfund.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>director@bluepilotfund.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>bobtrotman@gmail.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>peter.bober@gmail.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>markovangerven@gmail.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>drbonine@gmail.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>sbarry@bookpassage.com is not
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if christine@bookshopbenicia.com
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>ssahlein@aipb.org is not
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>brian.gallagher@unitedway.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if dgough@brand-agent.com
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if kshahane@brand-agent.com
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>lsieman@hotmail.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>elange@breproperties.com is not
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>david_smith@bridge-point.com is not
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>robert_andersen@bridge-point.com is not
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>sahjordan@yahoo.com is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>ekennett@nibs.org is
 a valid deliverable e-mail box address.</t>
   </si>
 </sst>
@@ -342,13 +702,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-  </numFmts>
-  <fonts count="22">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -364,159 +719,8 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="34">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -525,198 +729,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -739,251 +757,9 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="6" fontId="9" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="43">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="44">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="41">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="9">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="42">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="4" fillId="7" fontId="10" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="2" fillId="0" fontId="11" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyFont="0" applyNumberFormat="0" applyProtection="0" borderId="3" fillId="3" fontId="3" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="8" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="12" fontId="12" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="5" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="5" fontId="9" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="16" fontId="9" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="7" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="4" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="2" fillId="0" fontId="6" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="7" fillId="0" fontId="16" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="16" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="5" fillId="11" fontId="14" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="22" fontId="12" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="26" fontId="19" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="9" fillId="30" fontId="20" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="33" fontId="9" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="5" fillId="30" fontId="21" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="8" fillId="0" fontId="18" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="6" fillId="0" fontId="17" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="15" fontId="15" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="10" fontId="13" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="29" fontId="12" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="32" fontId="9" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="21" fontId="12" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="19" fontId="12" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="25" fontId="9" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="24" fontId="9" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="9" fontId="12" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="28" fontId="12" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="31" fontId="9" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="18" fontId="12" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="23" fontId="9" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="14" fontId="9" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="27" fontId="12" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="4" fontId="9" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="20" fontId="12" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="17" fontId="12" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="13" fontId="9" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="8" fontId="12" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
@@ -993,57 +769,10 @@
     </xf>
     <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
-    <cellStyle builtinId="31" name="40% - Accent1" xfId="1"/>
-    <cellStyle builtinId="3" name="Comma" xfId="2"/>
-    <cellStyle builtinId="4" name="Currency" xfId="3"/>
-    <cellStyle builtinId="6" name="Comma[0]" xfId="4"/>
-    <cellStyle builtinId="5" name="Percent" xfId="5"/>
-    <cellStyle builtinId="7" name="Currency[0]" xfId="6"/>
-    <cellStyle builtinId="23" name="Check Cell" xfId="7"/>
-    <cellStyle builtinId="17" name="Heading 2" xfId="8"/>
-    <cellStyle builtinId="10" name="Note" xfId="9"/>
-    <cellStyle builtinId="8" name="Hyperlink" xfId="10"/>
-    <cellStyle builtinId="44" name="60% - Accent4" xfId="11"/>
-    <cellStyle builtinId="9" name="Followed Hyperlink" xfId="12"/>
-    <cellStyle builtinId="39" name="40% - Accent3" xfId="13"/>
-    <cellStyle builtinId="11" name="Warning Text" xfId="14"/>
-    <cellStyle builtinId="35" name="40% - Accent2" xfId="15"/>
-    <cellStyle builtinId="15" name="Title" xfId="16"/>
-    <cellStyle builtinId="53" name="CExplanatory Text" xfId="17"/>
-    <cellStyle builtinId="16" name="Heading 1" xfId="18"/>
-    <cellStyle builtinId="18" name="Heading 3" xfId="19"/>
-    <cellStyle builtinId="19" name="Heading 4" xfId="20"/>
-    <cellStyle builtinId="20" name="Input" xfId="21"/>
-    <cellStyle builtinId="40" name="60% - Accent3" xfId="22"/>
-    <cellStyle builtinId="26" name="Good" xfId="23"/>
-    <cellStyle builtinId="21" name="Output" xfId="24"/>
-    <cellStyle builtinId="30" name="20% - Accent1" xfId="25"/>
-    <cellStyle builtinId="22" name="Calculation" xfId="26"/>
-    <cellStyle builtinId="24" name="Linked Cell" xfId="27"/>
-    <cellStyle builtinId="25" name="Total" xfId="28"/>
-    <cellStyle builtinId="27" name="Bad" xfId="29"/>
-    <cellStyle builtinId="28" name="Neutral" xfId="30"/>
-    <cellStyle builtinId="29" name="Accent1" xfId="31"/>
-    <cellStyle builtinId="46" name="20% - Accent5" xfId="32"/>
-    <cellStyle builtinId="32" name="60% - Accent1" xfId="33"/>
-    <cellStyle builtinId="33" name="Accent2" xfId="34"/>
-    <cellStyle builtinId="34" name="20% - Accent2" xfId="35"/>
-    <cellStyle builtinId="50" name="20% - Accent6" xfId="36"/>
-    <cellStyle builtinId="36" name="60% - Accent2" xfId="37"/>
-    <cellStyle builtinId="37" name="Accent3" xfId="38"/>
-    <cellStyle builtinId="38" name="20% - Accent3" xfId="39"/>
-    <cellStyle builtinId="41" name="Accent4" xfId="40"/>
-    <cellStyle builtinId="42" name="20% - Accent4" xfId="41"/>
-    <cellStyle builtinId="43" name="40% - Accent4" xfId="42"/>
-    <cellStyle builtinId="45" name="Accent5" xfId="43"/>
-    <cellStyle builtinId="47" name="40% - Accent5" xfId="44"/>
-    <cellStyle builtinId="48" name="60% - Accent5" xfId="45"/>
-    <cellStyle builtinId="49" name="Accent6" xfId="46"/>
-    <cellStyle builtinId="51" name="40% - Accent6" xfId="47"/>
-    <cellStyle builtinId="52" name="60% - Accent6" xfId="48"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
 </styleSheet>
 </file>
@@ -1305,18 +1034,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="A95" sqref="A95"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="39.1428571428571" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="108.142857142857" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="39.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="108.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row customFormat="1" r="1" s="1" spans="1:2">
@@ -1352,7 +1080,7 @@
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="3" t="s">
+      <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -1363,541 +1091,721 @@
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="3"/>
+      <c r="B6" s="3" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="3"/>
+      <c r="B7" s="3" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="3"/>
+      <c r="B8" s="3" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="3"/>
+      <c r="B9" s="3" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="3"/>
+      <c r="B10" s="3" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="3"/>
+      <c r="B11" s="3" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="3"/>
+      <c r="B12" s="3" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="3"/>
+      <c r="B13" s="3" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="3"/>
+      <c r="B14" s="3" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="3"/>
+      <c r="B15" s="3" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="3"/>
+      <c r="B16" s="3" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="3"/>
+      <c r="B17" s="3" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="3"/>
+      <c r="B18" s="3" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="3"/>
+      <c r="B19" s="3" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="3"/>
+      <c r="B20" s="3" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="3"/>
+      <c r="B21" s="3" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="3"/>
+      <c r="B22" s="3" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="3"/>
+      <c r="B23" s="3" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="3"/>
+      <c r="B24" s="3" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="3"/>
+      <c r="B25" s="3" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="3"/>
+      <c r="B26" s="3" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="3"/>
+      <c r="B27" s="3" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="3"/>
+      <c r="B28" s="3" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="3"/>
+      <c r="B29" s="3" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B30" s="3"/>
+      <c r="B30" s="3" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B31" s="3"/>
+      <c r="B31" s="3" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B32" s="3"/>
+      <c r="B32" s="3" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B33" s="3"/>
+      <c r="B33" s="3" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B34" s="3"/>
+      <c r="B34" s="3" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B35" s="3"/>
+      <c r="B35" s="3" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B36" s="3"/>
+      <c r="B36" s="3" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B37" s="3"/>
+      <c r="B37" s="3" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B38" s="3"/>
+      <c r="B38" s="3" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B39" s="3"/>
+      <c r="B39" s="3" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B40" s="3"/>
+      <c r="B40" s="3" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B41" s="3"/>
+      <c r="B41" s="3" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B42" s="3"/>
+      <c r="B42" s="3" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B43" s="3"/>
+      <c r="B43" s="3" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B44" s="3"/>
+      <c r="B44" s="3" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B45" s="3"/>
+      <c r="B45" s="3" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B46" s="3"/>
+      <c r="B46" s="3" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B47" s="3"/>
+      <c r="B47" s="3" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B48" s="3"/>
+      <c r="B48" s="3" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B49" s="3"/>
+      <c r="B49" s="3" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B50" s="3"/>
+      <c r="B50" s="3" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B51" s="3"/>
+      <c r="B51" s="3" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B52" s="3"/>
+      <c r="B52" s="3" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B53" s="3"/>
+      <c r="B53" s="3" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B54" s="3"/>
+      <c r="B54" s="3" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B55" s="3"/>
+      <c r="B55" s="3" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B56" s="3"/>
+      <c r="B56" s="3" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B57" s="3"/>
+      <c r="B57" s="3" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B58" s="3"/>
+      <c r="B58" s="3" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B59" s="3"/>
+      <c r="B59" s="3" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B60" s="3"/>
+      <c r="B60" s="3" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B61" s="3"/>
+      <c r="B61" s="3" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B62" s="3"/>
+      <c r="B62" s="3" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B63" s="3"/>
+      <c r="B63" s="3" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B64" s="3"/>
+      <c r="B64" s="3" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B65" s="3"/>
+      <c r="B65" s="3" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B66" s="3"/>
+      <c r="B66" s="3" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B67" s="3"/>
+      <c r="B67" s="3" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B68" s="3"/>
+      <c r="B68" s="3" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B69" s="3"/>
+      <c r="B69" s="3" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B70" s="3"/>
+      <c r="B70" s="3" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B71" s="3"/>
+      <c r="B71" s="3" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B72" s="3"/>
+      <c r="B72" s="3" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B73" s="3"/>
+      <c r="B73" s="3" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B74" s="3"/>
+      <c r="B74" s="3" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B75" s="3"/>
+      <c r="B75" s="3" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B76" s="3"/>
+      <c r="B76" s="3" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B77" s="3"/>
+      <c r="B77" s="3" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B78" s="3"/>
+      <c r="B78" s="3" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B79" s="3"/>
+      <c r="B79" s="3" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B80" s="3"/>
+      <c r="B80" s="3" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B81" s="3"/>
+      <c r="B81" s="3" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B82" s="3"/>
+      <c r="B82" s="3" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B83" s="3"/>
+      <c r="B83" s="3" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B84" s="3"/>
+      <c r="B84" s="3" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B85" s="3"/>
+      <c r="B85" s="3" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="B86" s="3"/>
+      <c r="B86" s="3" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="B87" s="3"/>
+      <c r="B87" s="3" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="B88" s="3"/>
+      <c r="B88" s="3" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="B89" s="3"/>
+      <c r="B89" s="3" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B90" s="3"/>
+      <c r="B90" s="3" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="91" spans="1:2">
       <c r="A91" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="B91" s="3"/>
+      <c r="B91" s="3" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="92" spans="1:2">
       <c r="A92" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="B92" s="3"/>
+      <c r="B92" s="3" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="93" spans="1:2">
       <c r="A93" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B93" s="3"/>
+      <c r="B93" s="3" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="94" spans="1:2">
       <c r="A94" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B94" s="3"/>
+      <c r="B94" s="3" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="95" spans="1:2">
       <c r="A95" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B95" s="3"/>
+      <c r="B95" s="3" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="96" spans="1:2">
       <c r="A96" s="3" t="s">
@@ -1936,8 +1844,10 @@
       <c r="B101" s="3"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.699305555555556" right="0.699305555555556" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="1"/>
-  <headerFooter/>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="A6"/>
+  </hyperlinks>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.69930555555555596" right="0.69930555555555596" top="0.75"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Committed on 27:02:2018:11:35:00AM By Karthikeyan Rajendran
</commit_message>
<xml_diff>
--- a/data/Mail_Campaign_One.xlsx
+++ b/data/Mail_Campaign_One.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\workspace\Ameex_Marketing_Team\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView windowHeight="8385" windowWidth="20385" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20385" windowHeight="8385"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="201">
   <si>
     <t>Email ID</t>
   </si>
@@ -695,14 +700,33 @@
   </si>
   <si>
     <t>ekennett@nibs.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>rcolker@nibs.org is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>pkmakin@Brilliant-Books.net is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>sara.grochowski@brilliant-books.net is
+a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>It was not possible to determine if mitch.simpson@brokawsupply.com
+is a valid deliverable e-mail box address.</t>
+  </si>
+  <si>
+    <t>mbrown@brownrichards.com is not
 a valid deliverable e-mail box address.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -759,21 +783,29 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -782,10 +814,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -949,21 +981,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -980,7 +1012,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -1034,20 +1066,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C101"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="A95" sqref="A95"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="39.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="108.140625" collapsed="true"/>
+    <col min="1" max="1" width="39.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="108.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="1" spans="1:2">
+    <row r="1" spans="1:2" s="1" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1811,31 +1841,41 @@
       <c r="A96" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B96" s="3"/>
+      <c r="B96" s="3" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="97" spans="1:2">
       <c r="A97" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B97" s="3"/>
+      <c r="B97" s="3" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="98" spans="1:2">
       <c r="A98" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="B98" s="3"/>
+      <c r="B98" s="3" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="99" spans="1:2">
       <c r="A99" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B99" s="3"/>
+      <c r="B99" s="3" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="100" spans="1:2">
       <c r="A100" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B100" s="3"/>
+      <c r="B100" s="3" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="101" spans="1:2">
       <c r="A101" s="3" t="s">
@@ -1845,9 +1885,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="A6"/>
+    <hyperlink ref="A6" r:id="rId1"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.69930555555555596" right="0.69930555555555596" top="0.75"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>